<commit_message>
Updated and fixed bugs
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/frc_asset_schedule.xlsx
+++ b/afar_project/csv_path/excel_files/frc_asset_schedule.xlsx
@@ -513,19 +513,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2214161.3</v>
+        <v>2214149.3</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2214161.3</v>
+        <v>2214149.3</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2214161.3</v>
+        <v>2214149.3</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -533,16 +533,16 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2000764.58</v>
+        <v>1761181.52</v>
       </c>
       <c r="J2" t="n">
-        <v>190486.86</v>
+        <v>239578.26</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>2191251.44</v>
+        <v>2000759.78</v>
       </c>
       <c r="M2" t="n">
         <v>0.04</v>
@@ -551,7 +551,7 @@
         <v>0.04</v>
       </c>
       <c r="O2" t="n">
-        <v>22909.82</v>
+        <v>213389.48</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2388974.43</v>
+        <v>2115213.29</v>
       </c>
       <c r="J3" t="n">
         <v>273761.14</v>
@@ -598,7 +598,7 @@
         <v>835243</v>
       </c>
       <c r="L3" t="n">
-        <v>1827492.57</v>
+        <v>1553731.43</v>
       </c>
       <c r="M3" t="n">
         <v>1200.06</v>
@@ -607,7 +607,7 @@
         <v>1900.06</v>
       </c>
       <c r="O3" t="n">
-        <v>86935.37</v>
+        <v>360696.51</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1410257.88</v>
+        <v>1235426.37</v>
       </c>
       <c r="J4" t="n">
         <v>174831.51</v>
@@ -654,7 +654,7 @@
         <v>426448.72</v>
       </c>
       <c r="L4" t="n">
-        <v>1158640.67</v>
+        <v>983809.16</v>
       </c>
       <c r="M4" t="n">
         <v>2587.59</v>
@@ -663,7 +663,7 @@
         <v>2587.59</v>
       </c>
       <c r="O4" t="n">
-        <v>587086.88</v>
+        <v>761918.39</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>284157.14</v>
+        <v>236352.14</v>
       </c>
       <c r="J5" t="n">
         <v>47805</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>331962.14</v>
+        <v>284157.14</v>
       </c>
       <c r="M5" t="n">
         <v>0.03</v>
@@ -719,7 +719,7 @@
         <v>0.03</v>
       </c>
       <c r="O5" t="n">
-        <v>2672.83</v>
+        <v>50477.83</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>11999348.1</v>
+        <v>9831338.699999999</v>
       </c>
       <c r="J6" t="n">
         <v>2168009.4</v>
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>14167357.5</v>
+        <v>11999348.1</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>7512736.5</v>
+        <v>9680745.9</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>82394.75999999999</v>
+        <v>54929.84</v>
       </c>
       <c r="J7" t="n">
         <v>27464.92</v>
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>109859.68</v>
+        <v>82394.75999999999</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>439438.52</v>
+        <v>466903.44</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>143670.96</v>
+        <v>95780.64</v>
       </c>
       <c r="J8" t="n">
         <v>47890.32</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>191561.28</v>
+        <v>143670.96</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>526793.72</v>
+        <v>574684.04</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>13380</v>
+        <v>8920</v>
       </c>
       <c r="J9" t="n">
         <v>4460</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>17840</v>
+        <v>13380</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>49060</v>
+        <v>53520</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>91178.25</v>
+        <v>60785.5</v>
       </c>
       <c r="J10" t="n">
         <v>30392.75</v>
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>121571</v>
+        <v>91178.25</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>486284</v>
+        <v>516676.75</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -1020,16 +1020,16 @@
         <v>1402841.25</v>
       </c>
       <c r="D11" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1402859.25</v>
+        <v>1402841.25</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1402859.25</v>
+        <v>1402841.25</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1037,16 +1037,16 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>280569.48</v>
+        <v>187045.52</v>
       </c>
       <c r="J11" t="n">
-        <v>93523.96000000001</v>
+        <v>93522.75999999999</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>374093.44</v>
+        <v>280568.28</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>1028765.81</v>
+        <v>1122272.97</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>112790.64</v>
+        <v>75193.75999999999</v>
       </c>
       <c r="J12" t="n">
         <v>37596.88</v>
@@ -1102,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>150387.52</v>
+        <v>112790.64</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>225581.23</v>
+        <v>263178.11</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>709991.97</v>
+        <v>473327.98</v>
       </c>
       <c r="J13" t="n">
         <v>236663.99</v>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>946655.96</v>
+        <v>709991.97</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>3786623.29</v>
+        <v>4023287.28</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>954222.89</v>
+        <v>636143.62</v>
       </c>
       <c r="J14" t="n">
         <v>318079.27</v>
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>1272302.16</v>
+        <v>954222.89</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>3498887.34</v>
+        <v>3816966.61</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>

</xml_diff>